<commit_message>
Production mode works but not pagination
</commit_message>
<xml_diff>
--- a/YouTube-Comment-Analyzer-Complete.xlsx
+++ b/YouTube-Comment-Analyzer-Complete.xlsx
@@ -65,11 +65,11 @@
     </font>
     <font>
       <b val="1"/>
-      <color rgb="00FF0000"/>
+      <color rgb="00787878"/>
     </font>
     <font>
       <b val="1"/>
-      <color rgb="00787878"/>
+      <color rgb="00FF0000"/>
     </font>
     <font/>
     <font>
@@ -144,7 +144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -153,7 +153,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -178,7 +178,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -569,7 +569,7 @@
       </c>
       <c r="B1" s="4" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=FOqICW5-zgw&amp;ab_channel=TheWildAnimalChannel</t>
+          <t>Nat Geo Wild - The Life Of The Pythons - National Geographic</t>
         </is>
       </c>
     </row>
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="B2" s="7" t="n">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3"/>
@@ -591,11 +591,11 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" s="9" t="inlineStr">
         <is>
-          <t>60.0%</t>
+          <t>14.634146341463415%</t>
         </is>
       </c>
     </row>
@@ -606,11 +606,11 @@
         </is>
       </c>
       <c r="B5" s="11" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C5" s="11" t="inlineStr">
         <is>
-          <t>20.0%</t>
+          <t>26.829268292682926%</t>
         </is>
       </c>
     </row>
@@ -621,11 +621,11 @@
         </is>
       </c>
       <c r="B6" s="13" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C6" s="13" t="inlineStr">
         <is>
-          <t>20.0%</t>
+          <t>58.53658536585366%</t>
         </is>
       </c>
     </row>
@@ -647,7 +647,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -670,7 +670,7 @@
       </c>
       <c r="B1" s="15" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=FOqICW5-zgw&amp;ab_channel=TheWildAnimalChannel</t>
+          <t>Nat Geo Wild - The Life Of The Pythons - National Geographic</t>
         </is>
       </c>
     </row>
@@ -704,7 +704,7 @@
     <row r="3">
       <c r="A3" s="18" t="inlineStr">
         <is>
-          <t>2021-01-01</t>
+          <t>2022-07-13</t>
         </is>
       </c>
       <c r="B3" s="9" t="inlineStr">
@@ -713,23 +713,23 @@
         </is>
       </c>
       <c r="C3" s="18" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3" s="18" t="inlineStr">
         <is>
-          <t>User1</t>
+          <t>@johnschultz8906</t>
         </is>
       </c>
       <c r="E3" s="19" t="inlineStr">
         <is>
-          <t>Great video!</t>
+          <t>I never new gators hide food underwater so it's easier to tear apart that's amazing</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="18" t="inlineStr">
         <is>
-          <t>2021-01-02</t>
+          <t>2021-01-31</t>
         </is>
       </c>
       <c r="B4" s="9" t="inlineStr">
@@ -738,23 +738,23 @@
         </is>
       </c>
       <c r="C4" s="18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="18" t="inlineStr">
         <is>
-          <t>User2</t>
+          <t>@NaturestoursTV</t>
         </is>
       </c>
       <c r="E4" s="19" t="inlineStr">
         <is>
-          <t>Very informative.</t>
+          <t>Good video 😊 needs a python thumb nail not ball python big misslead and size difference</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="18" t="inlineStr">
         <is>
-          <t>2021-01-04</t>
+          <t>2020-08-17</t>
         </is>
       </c>
       <c r="B5" s="9" t="inlineStr">
@@ -763,16 +763,91 @@
         </is>
       </c>
       <c r="C5" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="18" t="inlineStr">
+        <is>
+          <t>@ilovebluegrass5493</t>
+        </is>
+      </c>
+      <c r="E5" s="19" t="inlineStr">
+        <is>
+          <t>Oh I just love snakes I want to be a snake breeder</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="18" t="inlineStr">
+        <is>
+          <t>2020-07-21</t>
+        </is>
+      </c>
+      <c r="B6" s="9" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="C6" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="18" t="inlineStr">
-        <is>
-          <t>User4</t>
-        </is>
-      </c>
-      <c r="E5" s="19" t="inlineStr">
-        <is>
-          <t>It was ok.</t>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>@verdeslam44</t>
+        </is>
+      </c>
+      <c r="E6" s="19" t="inlineStr">
+        <is>
+          <t>@25:05  Biologist lady: "Good girl!" as she feeds the endangered Wood Rat with enormous ball sack.😁</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="18" t="inlineStr">
+        <is>
+          <t>2020-03-04</t>
+        </is>
+      </c>
+      <c r="B7" s="9" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="C7" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
+        <is>
+          <t>@siearrawebb7048</t>
+        </is>
+      </c>
+      <c r="E7" s="19" t="inlineStr">
+        <is>
+          <t>I see he brought his grandmas pillowcase for this trip. Lol 😆</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="18" t="inlineStr">
+        <is>
+          <t>2017-10-14</t>
+        </is>
+      </c>
+      <c r="B8" s="9" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="C8" s="18" t="n">
+        <v>41</v>
+      </c>
+      <c r="D8" s="18" t="inlineStr">
+        <is>
+          <t>@foodathlete1685</t>
+        </is>
+      </c>
+      <c r="E8" s="19" t="inlineStr">
+        <is>
+          <t>I like how homeboy just goes around snatching up pythons 😂😂</t>
         </is>
       </c>
     </row>
@@ -790,7 +865,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -813,7 +888,7 @@
       </c>
       <c r="B1" s="15" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=FOqICW5-zgw&amp;ab_channel=TheWildAnimalChannel</t>
+          <t>Nat Geo Wild - The Life Of The Pythons - National Geographic</t>
         </is>
       </c>
     </row>
@@ -847,7 +922,7 @@
     <row r="3">
       <c r="A3" s="18" t="inlineStr">
         <is>
-          <t>2020-01-04</t>
+          <t>2022-06-25</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
@@ -860,12 +935,264 @@
       </c>
       <c r="D3" s="18" t="inlineStr">
         <is>
-          <t>User5</t>
+          <t>@robertobezerra1766</t>
         </is>
       </c>
       <c r="E3" s="19" t="inlineStr">
         <is>
-          <t>This video in on YouTube.</t>
+          <t>As Duas MAIORES espécies de Serpentes do Mundo e tbm as Mais Pesadas, São a ( Píton Reticulada e a Sucuri, tbm Chamada em alguns Países da América do Sul de Anaconda. ) são da família das Cobras Constritoras (que sufocam suas presas para matar), Cobras Constritoras usam seu próprio Corpo como arma de Combate, envolvendo a vítima e esmagando-a, até que o coração da presa pare de bater e/ou a respiração cesse. o abraço destas cobras tbm Conhecido como “abraço-da-morte” supera os 150 kg, a mais forte passa dos</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="18" t="inlineStr">
+        <is>
+          <t>2022-06-25</t>
+        </is>
+      </c>
+      <c r="B4" s="11" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="C4" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="18" t="inlineStr">
+        <is>
+          <t>@robertobezerra1766</t>
+        </is>
+      </c>
+      <c r="E4" s="19" t="inlineStr">
+        <is>
+          <t>a Famosa Píton Birmanesa tbm Conhecida como Píton Burmesa, nome Científico ( Python bivittatus ). é minha Favorita Das espécies Grandes Serpentes, Pois além de ser a mais bonita tbm É Considerada a mais dócil e mansa das Grandes Cobras. a Píton Birmanesa é a 5°Quinta MAIOR espécie de Cobra em Comprimento, podendo atingir um tamanho Entre ( 04,32 mc, à 05,00 m, ) de Comprimento. OBS: de Acordo com a ( Herpetologia ) a Ciência que estuda os anfíbios e répteis. algumas Cobras da espécie Píton Birmanesa podem c</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="18" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="B5" s="11" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="C5" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="18" t="inlineStr">
+        <is>
+          <t>@robertobezerra1766</t>
+        </is>
+      </c>
+      <c r="E5" s="19" t="inlineStr">
+        <is>
+          <t>Amo Muito os Animais 🙂 Girafas, Ursos, Lobos, Rinocerontes, Leopardos, Suricatos, o Ratel, o Carcaju, o Gato-Maracajá, o Feneco, o Cachorro Vinagre, o Macaco Orangotango, o Tamanduá-Bandeira, o Elande, Zebras, Cavalos Selvagens, o Calau, o Lagarto Varano-do-Nilo, a grande Serpente Píton Birmanesa e etc. mais os meus DOIS Animais Preferidos são o Hipopótamo e o Cachorro Selvagem Africano. O nome Hipopótamo provêm do Grego Antigo, e Significa "Cavalo do Rio". gosto muito dos Hipopótamos e Não pela beleza, poi</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="18" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="B6" s="11" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="C6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>@robertobezerra1766</t>
+        </is>
+      </c>
+      <c r="E6" s="19" t="inlineStr">
+        <is>
+          <t>As Duas MAIORES espécies de Serpentes do Mundo e tbm as Mais Pesadas, São a ( Píton Reticulada e a Sucuri, tbm Chamada em alguns Países da América do Sul de Anaconda. ) são da família das Cobras Constritoras (que sufocam suas presas para matar), Cobras Constritoras usam seu próprio Corpo como arma de Combate, envolvendo a vítima e esmagando-a, até que o coração da presa pare de bater e/ou a respiração cesse. o abraço destas cobras tbm Conhecido como “abraço-da-morte” supera os 150 kg, a mais forte passa dos</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="18" t="inlineStr">
+        <is>
+          <t>2022-03-30</t>
+        </is>
+      </c>
+      <c r="B7" s="11" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="C7" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
+        <is>
+          <t>@raeedbrown8532</t>
+        </is>
+      </c>
+      <c r="E7" s="19" t="inlineStr">
+        <is>
+          <t>Feed them to king cobras</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="18" t="inlineStr">
+        <is>
+          <t>2020-12-13</t>
+        </is>
+      </c>
+      <c r="B8" s="11" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="C8" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="18" t="inlineStr">
+        <is>
+          <t>@danielskerman1343</t>
+        </is>
+      </c>
+      <c r="E8" s="19" t="inlineStr">
+        <is>
+          <t>13:58
+O L L I G A T O R</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="18" t="inlineStr">
+        <is>
+          <t>2020-08-16</t>
+        </is>
+      </c>
+      <c r="B9" s="11" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="C9" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="18" t="inlineStr">
+        <is>
+          <t>@avatarswife78</t>
+        </is>
+      </c>
+      <c r="E9" s="19" t="inlineStr">
+        <is>
+          <t>Why don't they ship them back to their natural habitat?</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="18" t="inlineStr">
+        <is>
+          <t>2020-08-13</t>
+        </is>
+      </c>
+      <c r="B10" s="11" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="C10" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="18" t="inlineStr">
+        <is>
+          <t>@tekksavvy2242</t>
+        </is>
+      </c>
+      <c r="E10" s="19" t="inlineStr">
+        <is>
+          <t>!</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="18" t="inlineStr">
+        <is>
+          <t>2020-06-11</t>
+        </is>
+      </c>
+      <c r="B11" s="11" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="C11" s="18" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" s="18" t="inlineStr">
+        <is>
+          <t>@nqnguyen2008</t>
+        </is>
+      </c>
+      <c r="E11" s="19" t="inlineStr">
+        <is>
+          <t>I have no idea why, but I kinda want a snake as a pet, a friendly snaje of course. I could scare
+my cousin with it. She scared of smakes. My mom would be scared too.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="18" t="inlineStr">
+        <is>
+          <t>2019-09-02</t>
+        </is>
+      </c>
+      <c r="B12" s="11" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="C12" s="18" t="n">
+        <v>7</v>
+      </c>
+      <c r="D12" s="18" t="inlineStr">
+        <is>
+          <t>@eternal_napalm6442</t>
+        </is>
+      </c>
+      <c r="E12" s="19" t="inlineStr">
+        <is>
+          <t>Ball Python in thumbnail and no Ball Pythons.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="18" t="inlineStr">
+        <is>
+          <t>2019-06-18</t>
+        </is>
+      </c>
+      <c r="B13" s="11" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="C13" s="18" t="n">
+        <v>7</v>
+      </c>
+      <c r="D13" s="18" t="inlineStr">
+        <is>
+          <t>@elijahmiller6187</t>
+        </is>
+      </c>
+      <c r="E13" s="19" t="inlineStr">
+        <is>
+          <t>I have a feeling that Burm didn't meet that indigo by chance</t>
         </is>
       </c>
     </row>
@@ -883,7 +1210,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -906,7 +1233,7 @@
       </c>
       <c r="B1" s="15" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=FOqICW5-zgw&amp;ab_channel=TheWildAnimalChannel</t>
+          <t>Nat Geo Wild - The Life Of The Pythons - National Geographic</t>
         </is>
       </c>
     </row>
@@ -940,7 +1267,7 @@
     <row r="3">
       <c r="A3" s="18" t="inlineStr">
         <is>
-          <t>2021-01-03</t>
+          <t>2022-06-16</t>
         </is>
       </c>
       <c r="B3" s="20" t="inlineStr">
@@ -949,16 +1276,593 @@
         </is>
       </c>
       <c r="C3" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="18" t="inlineStr">
+        <is>
+          <t>@CG-ry9ne</t>
+        </is>
+      </c>
+      <c r="E3" s="19" t="inlineStr">
+        <is>
+          <t>This comment goes out to the rat in the bait box. Homie be livin in fear 24/7</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="18" t="inlineStr">
+        <is>
+          <t>2021-05-17</t>
+        </is>
+      </c>
+      <c r="B4" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C4" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="18" t="inlineStr">
+        <is>
+          <t>@haryakshshah4936</t>
+        </is>
+      </c>
+      <c r="E4" s="19" t="inlineStr">
+        <is>
+          <t>It’s not a good idea to kill snakes like that. They need to be transferred to their natural habitat in Asia a comfortable and safe manner if they’re causing harm. Do,estimated ownership of snakes needs to be prohibited</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="18" t="inlineStr">
+        <is>
+          <t>2020-12-05</t>
+        </is>
+      </c>
+      <c r="B5" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C5" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="18" t="inlineStr">
+        <is>
+          <t>@silvirhunter3607</t>
+        </is>
+      </c>
+      <c r="E5" s="19" t="inlineStr">
+        <is>
+          <t>These beautiful creatures shouldn't be eradicated in my opinion,  reduced populations I can agree with, but wiping them out entirely? No, I don't think so. Just my opinion.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="18" t="inlineStr">
+        <is>
+          <t>2020-08-06</t>
+        </is>
+      </c>
+      <c r="B6" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C6" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>@davidjr3769</t>
+        </is>
+      </c>
+      <c r="E6" s="19" t="inlineStr">
+        <is>
+          <t>Worst thing you can do is release a pet , better of killing it if you can’t find it a home ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="18" t="inlineStr">
+        <is>
+          <t>2020-07-19</t>
+        </is>
+      </c>
+      <c r="B7" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C7" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="18" t="inlineStr">
-        <is>
-          <t>User3</t>
-        </is>
-      </c>
-      <c r="E3" s="19" t="inlineStr">
-        <is>
-          <t>Not great.</t>
+      <c r="D7" s="18" t="inlineStr">
+        <is>
+          <t>@juliangoodman5046</t>
+        </is>
+      </c>
+      <c r="E7" s="19" t="inlineStr">
+        <is>
+          <t>I swear snakes are retarted , they eyes are good for nothing .</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="18" t="inlineStr">
+        <is>
+          <t>2020-07-18</t>
+        </is>
+      </c>
+      <c r="B8" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C8" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="18" t="inlineStr">
+        <is>
+          <t>@zacksparrow340</t>
+        </is>
+      </c>
+      <c r="E8" s="19" t="inlineStr">
+        <is>
+          <t>Clearly postmortem of python if it is dead its go but if you killed it you guys sucks</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="18" t="inlineStr">
+        <is>
+          <t>2020-07-18</t>
+        </is>
+      </c>
+      <c r="B9" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C9" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="18" t="inlineStr">
+        <is>
+          <t>@zacksparrow340</t>
+        </is>
+      </c>
+      <c r="E9" s="19" t="inlineStr">
+        <is>
+          <t>Dont kill them crab</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="18" t="inlineStr">
+        <is>
+          <t>2020-07-12</t>
+        </is>
+      </c>
+      <c r="B10" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C10" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" s="18" t="inlineStr">
+        <is>
+          <t>@crystalm4324</t>
+        </is>
+      </c>
+      <c r="E10" s="19" t="inlineStr">
+        <is>
+          <t>14:35 why the heck is he calling them Ollygators??? If I worked with him, or had him for a professor, I’d go nuts!!
+AL LI GA TOR!!  
+Someone needs to teach him Syllaulibles🤣🤣🤣</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="18" t="inlineStr">
+        <is>
+          <t>2020-05-24</t>
+        </is>
+      </c>
+      <c r="B11" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C11" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" s="18" t="inlineStr">
+        <is>
+          <t>@theflyingdutchman7969</t>
+        </is>
+      </c>
+      <c r="E11" s="19" t="inlineStr">
+        <is>
+          <t>That python must be so confused after biting the balloon🤣</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="18" t="inlineStr">
+        <is>
+          <t>2020-04-22</t>
+        </is>
+      </c>
+      <c r="B12" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C12" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="18" t="inlineStr">
+        <is>
+          <t>@MrDopestDope1</t>
+        </is>
+      </c>
+      <c r="E12" s="19" t="inlineStr">
+        <is>
+          <t>if this budget was spent on prevention of disease then corona would not have hit us like this</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="18" t="inlineStr">
+        <is>
+          <t>2020-03-21</t>
+        </is>
+      </c>
+      <c r="B13" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C13" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" s="18" t="inlineStr">
+        <is>
+          <t>@seekinghisface7762</t>
+        </is>
+      </c>
+      <c r="E13" s="19" t="inlineStr">
+        <is>
+          <t>If you put them in your menu... it will definitely make them endangered in the U.S.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="18" t="inlineStr">
+        <is>
+          <t>2020-02-29</t>
+        </is>
+      </c>
+      <c r="B14" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C14" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="18" t="inlineStr">
+        <is>
+          <t>@ElectricBlade</t>
+        </is>
+      </c>
+      <c r="E14" s="19" t="inlineStr">
+        <is>
+          <t>I love it how people in Florida like getting Exotic Animals  aka wild animals people wtf.... ohhh he just bit my wife's finger.... really boy you lucky it didnt bite your butt. Pythons??? People come on why not a cat and dog or fine a parrot but dont fckin think oh it's very nice nooo it's a responsibility and other than making yourself feel good they dont like living in your home they would rather have the wild life. Seriously what is it with people and trying to have wild pets... dont play god people resp</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="18" t="inlineStr">
+        <is>
+          <t>2020-01-24</t>
+        </is>
+      </c>
+      <c r="B15" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C15" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="18" t="inlineStr">
+        <is>
+          <t>@samuelwilliams5161</t>
+        </is>
+      </c>
+      <c r="E15" s="19" t="inlineStr">
+        <is>
+          <t>This is like immigration they leaving their shitty lives back home for the us</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="18" t="inlineStr">
+        <is>
+          <t>2020-01-14</t>
+        </is>
+      </c>
+      <c r="B16" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C16" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="18" t="inlineStr">
+        <is>
+          <t>@nickybanks3623</t>
+        </is>
+      </c>
+      <c r="E16" s="19" t="inlineStr">
+        <is>
+          <t>Animal rights those "scientists" should be cut open. I want to know that woman's mating routine</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="18" t="inlineStr">
+        <is>
+          <t>2019-12-04</t>
+        </is>
+      </c>
+      <c r="B17" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C17" s="18" t="n">
+        <v>16</v>
+      </c>
+      <c r="D17" s="18" t="inlineStr">
+        <is>
+          <t>@cornmon</t>
+        </is>
+      </c>
+      <c r="E17" s="19" t="inlineStr">
+        <is>
+          <t>It saddens me to see them manhandling these snakes. I especially dislike seeing how they handled the test python so shortly after it had eaten. This is terrifying for the snake, and it will probably regurgitate it's meal and go on a fast from this.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="18" t="inlineStr">
+        <is>
+          <t>2019-09-05</t>
+        </is>
+      </c>
+      <c r="B18" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C18" s="18" t="n">
+        <v>3</v>
+      </c>
+      <c r="D18" s="18" t="inlineStr">
+        <is>
+          <t>@x9466x</t>
+        </is>
+      </c>
+      <c r="E18" s="19" t="inlineStr">
+        <is>
+          <t>37:12 even the snake is 'tired' of their bad acting</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="18" t="inlineStr">
+        <is>
+          <t>2019-06-27</t>
+        </is>
+      </c>
+      <c r="B19" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C19" s="18" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" s="18" t="inlineStr">
+        <is>
+          <t>@neroknight1234</t>
+        </is>
+      </c>
+      <c r="E19" s="19" t="inlineStr">
+        <is>
+          <t>3:09 that terrible acting. Im sure you didnt put the snake there too....</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="18" t="inlineStr">
+        <is>
+          <t>2019-06-18</t>
+        </is>
+      </c>
+      <c r="B20" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C20" s="18" t="n">
+        <v>19</v>
+      </c>
+      <c r="D20" s="18" t="inlineStr">
+        <is>
+          <t>@elijahmiller6187</t>
+        </is>
+      </c>
+      <c r="E20" s="19" t="inlineStr">
+        <is>
+          <t>The way they handle these snakes is a little rough sometimes</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="18" t="inlineStr">
+        <is>
+          <t>2019-05-09</t>
+        </is>
+      </c>
+      <c r="B21" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C21" s="18" t="n">
+        <v>12</v>
+      </c>
+      <c r="D21" s="18" t="inlineStr">
+        <is>
+          <t>@gastonbell108</t>
+        </is>
+      </c>
+      <c r="E21" s="19" t="inlineStr">
+        <is>
+          <t>Python's teeth are not for poisoning you. They're for grabbing on to you so he can strangle the life out of you with the rest of his body.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="18" t="inlineStr">
+        <is>
+          <t>2019-04-15</t>
+        </is>
+      </c>
+      <c r="B22" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C22" s="18" t="n">
+        <v>12</v>
+      </c>
+      <c r="D22" s="18" t="inlineStr">
+        <is>
+          <t>@melissaleigh9119</t>
+        </is>
+      </c>
+      <c r="E22" s="19" t="inlineStr">
+        <is>
+          <t>Some of this was either staged or... nah it was staged. The acting is just too bad.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="18" t="inlineStr">
+        <is>
+          <t>2019-04-12</t>
+        </is>
+      </c>
+      <c r="B23" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C23" s="18" t="n">
+        <v>59</v>
+      </c>
+      <c r="D23" s="18" t="inlineStr">
+        <is>
+          <t>@TheCharleseye</t>
+        </is>
+      </c>
+      <c r="E23" s="19" t="inlineStr">
+        <is>
+          <t>I mean...but why use a picture of a captive bred Ball Python as the thumbnail? Seems a bit misleading, don't you think?</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="18" t="inlineStr">
+        <is>
+          <t>2019-02-24</t>
+        </is>
+      </c>
+      <c r="B24" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C24" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="18" t="inlineStr">
+        <is>
+          <t>@ApatheticBlogger</t>
+        </is>
+      </c>
+      <c r="E24" s="19" t="inlineStr">
+        <is>
+          <t>I love how they just fucking released a python into a river of crocodiles ,how the fuck is that not illegal</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="18" t="inlineStr">
+        <is>
+          <t>2019-02-14</t>
+        </is>
+      </c>
+      <c r="B25" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C25" s="18" t="n">
+        <v>26</v>
+      </c>
+      <c r="D25" s="18" t="inlineStr">
+        <is>
+          <t>@lsuhillary</t>
+        </is>
+      </c>
+      <c r="E25" s="19" t="inlineStr">
+        <is>
+          <t>They don’t suffocate their prey. The squeeze so tightly that the blood can no longer circulate. This makes the heart stop and the brain bleed. Suffocation takes much longer than a heart attack.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="18" t="inlineStr">
+        <is>
+          <t>2019-01-20</t>
+        </is>
+      </c>
+      <c r="B26" s="20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="C26" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="D26" s="18" t="inlineStr">
+        <is>
+          <t>@krumbers</t>
+        </is>
+      </c>
+      <c r="E26" s="19" t="inlineStr">
+        <is>
+          <t>O L L I G A T O R</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix error in README
</commit_message>
<xml_diff>
--- a/YouTube-Comment-Analyzer-Complete.xlsx
+++ b/YouTube-Comment-Analyzer-Complete.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="24" windowWidth="12900" windowHeight="12216" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Positive Comments" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Neutral Comments" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Negative Comments" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Positive" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Neutral" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Negative" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -39,14 +39,6 @@
       <sz val="11"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="10"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b val="1"/>
       <color rgb="00FFFFFF"/>
     </font>
@@ -61,27 +53,27 @@
     </font>
     <font>
       <b val="1"/>
+      <color rgb="00787878"/>
+    </font>
+    <font>
+      <b val="1"/>
       <color rgb="00FF0000"/>
     </font>
+    <font/>
     <font>
       <b val="1"/>
-      <color rgb="00787878"/>
+      <color rgb="00000000"/>
     </font>
     <font>
       <b val="1"/>
       <color rgb="00008000"/>
     </font>
-    <font/>
-    <font>
-      <b val="1"/>
-      <color rgb="00000000"/>
-    </font>
     <font>
       <b val="1"/>
       <color rgb="00C70039"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill/>
     </fill>
@@ -110,11 +102,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00008000"/>
       </patternFill>
     </fill>
@@ -138,58 +125,58 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -555,7 +542,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -572,9 +559,9 @@
           <t>YouTube Video:</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>Austin's Deep Trek Into The Jungle! 🕷😱 | Austin Steven's Adventures | Curious?: Natural World</t>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Pythons 101 | National Geographic</t>
         </is>
       </c>
     </row>
@@ -585,7 +572,7 @@
         </is>
       </c>
       <c r="B2" s="7" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3"/>
@@ -596,11 +583,11 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4" s="9" t="inlineStr">
         <is>
-          <t>25.0%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -615,7 +602,7 @@
       </c>
       <c r="C5" s="11" t="inlineStr">
         <is>
-          <t>33.3%</t>
+          <t>80.0%</t>
         </is>
       </c>
     </row>
@@ -626,11 +613,11 @@
         </is>
       </c>
       <c r="B6" s="13" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C6" s="13" t="inlineStr">
         <is>
-          <t>41.7%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -649,7 +636,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -661,7 +648,7 @@
     <col width="15" customWidth="1" style="4" min="2" max="2"/>
     <col width="15" customWidth="1" style="4" min="3" max="3"/>
     <col width="15" customWidth="1" style="4" min="4" max="4"/>
-    <col width="200" customWidth="1" style="4" min="5" max="5"/>
+    <col width="50" customWidth="1" style="4" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -672,7 +659,7 @@
       </c>
       <c r="B1" s="15" t="inlineStr">
         <is>
-          <t>Austin's Deep Trek Into The Jungle! 🕷😱 | Austin Steven's Adventures | Curious?: Natural World</t>
+          <t>Pythons 101 | National Geographic</t>
         </is>
       </c>
     </row>
@@ -700,81 +687,6 @@
       <c r="E2" s="17" t="inlineStr">
         <is>
           <t>Comment</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="18" t="inlineStr">
-        <is>
-          <t>2023-03-05</t>
-        </is>
-      </c>
-      <c r="B3" s="9" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="C3" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="18" t="inlineStr">
-        <is>
-          <t>@user-wr4ox3jt2h</t>
-        </is>
-      </c>
-      <c r="E3" s="19" t="inlineStr">
-        <is>
-          <t>With love and Respect Austin Stevens Thank you  All  La  Vita e Bella</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="18" t="inlineStr">
-        <is>
-          <t>2022-08-28</t>
-        </is>
-      </c>
-      <c r="B4" s="9" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="C4" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="18" t="inlineStr">
-        <is>
-          <t>@mrkipling2201</t>
-        </is>
-      </c>
-      <c r="E4" s="19" t="inlineStr">
-        <is>
-          <t>What nice people in that village. Even if the snake bite remedy doesn’t work, it can’t do any harm either and it shows respect to take it.  Great documentary. I’ve always loved his programmes. Jus wondered why the village chief had loads of bags of cement in the hut??</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="18" t="inlineStr">
-        <is>
-          <t>2022-06-09</t>
-        </is>
-      </c>
-      <c r="B5" s="9" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="C5" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" s="18" t="inlineStr">
-        <is>
-          <t>@alvaroalcantara969</t>
-        </is>
-      </c>
-      <c r="E5" s="19" t="inlineStr">
-        <is>
-          <t>This dude is a legend</t>
         </is>
       </c>
     </row>
@@ -804,7 +716,7 @@
     <col width="15" customWidth="1" style="4" min="2" max="2"/>
     <col width="15" customWidth="1" style="4" min="3" max="3"/>
     <col width="15" customWidth="1" style="4" min="4" max="4"/>
-    <col width="200" customWidth="1" style="4" min="5" max="5"/>
+    <col width="50" customWidth="1" style="4" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -815,7 +727,7 @@
       </c>
       <c r="B1" s="15" t="inlineStr">
         <is>
-          <t>Austin's Deep Trek Into The Jungle! 🕷😱 | Austin Steven's Adventures | Curious?: Natural World</t>
+          <t>Pythons 101 | National Geographic</t>
         </is>
       </c>
     </row>
@@ -849,7 +761,7 @@
     <row r="3">
       <c r="A3" s="18" t="inlineStr">
         <is>
-          <t>2023-12-01</t>
+          <t>2018-03-20</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
@@ -858,23 +770,23 @@
         </is>
       </c>
       <c r="C3" s="18" t="n">
-        <v>0</v>
+        <v>199</v>
       </c>
       <c r="D3" s="18" t="inlineStr">
         <is>
-          <t>@kagamiuchiha25</t>
+          <t>@NatGeo</t>
         </is>
       </c>
       <c r="E3" s="19" t="inlineStr">
         <is>
-          <t>Tzabcan rattlesnake is also called the Yucatan Neotropical Rattlesnake. I wonder if its venom is more potent than any other species of rattlesnake including WDB.</t>
+          <t>While pythons can typically grow up to be 200 pounds, a 403-pound Burmese python named Baby currently holds the record for the heaviest snake in captivity. What's your favorite python fact from this video?</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="18" t="inlineStr">
         <is>
-          <t>2023-05-17</t>
+          <t>2023-10-25</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
@@ -883,23 +795,23 @@
         </is>
       </c>
       <c r="C4" s="18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4" s="18" t="inlineStr">
         <is>
-          <t>@trumanhw</t>
+          <t>@obryan240</t>
         </is>
       </c>
       <c r="E4" s="19" t="inlineStr">
         <is>
-          <t>anyone notice that first lancehead he found he "moved to keep someone from being bitten by it" ...he moved all of about 6 feet away? lol.</t>
+          <t>One of these "pythons" shown was a boa.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="18" t="inlineStr">
         <is>
-          <t>2022-06-09</t>
+          <t>2023-09-01</t>
         </is>
       </c>
       <c r="B5" s="11" t="inlineStr">
@@ -908,23 +820,23 @@
         </is>
       </c>
       <c r="C5" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="18" t="inlineStr">
         <is>
-          <t>@tooldtoscold6687</t>
+          <t>@windioktavia6394</t>
         </is>
       </c>
       <c r="E5" s="19" t="inlineStr">
         <is>
-          <t>I wonder what his life insurance premiums are ?</t>
+          <t>Hallo..I'm windi oktavia from shandhika widya cinema the keajaiban dunia program Net TV. Want to ask for this account video and permission to play the net TV kejaiaban dunia program, and then we'll include a source/credit title with this account name, thank you</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="18" t="inlineStr">
         <is>
-          <t>2022-06-09</t>
+          <t>2023-06-17</t>
         </is>
       </c>
       <c r="B6" s="11" t="inlineStr">
@@ -933,16 +845,16 @@
         </is>
       </c>
       <c r="C6" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="18" t="inlineStr">
         <is>
-          <t>@CuriousNaturalWorld</t>
+          <t>@EJ-kk5mw</t>
         </is>
       </c>
       <c r="E6" s="19" t="inlineStr">
         <is>
-          <t>Want to see more of Austin Steven's Adventures? 🕷 Watch full episodes here: https://bit.ly/3mV2n8r</t>
+          <t>why pythons have legs?</t>
         </is>
       </c>
     </row>
@@ -960,7 +872,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -972,7 +884,7 @@
     <col width="15" customWidth="1" style="4" min="2" max="2"/>
     <col width="15" customWidth="1" style="4" min="3" max="3"/>
     <col width="15" customWidth="1" style="4" min="4" max="4"/>
-    <col width="200" customWidth="1" style="4" min="5" max="5"/>
+    <col width="50" customWidth="1" style="4" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -983,7 +895,7 @@
       </c>
       <c r="B1" s="15" t="inlineStr">
         <is>
-          <t>Austin's Deep Trek Into The Jungle! 🕷😱 | Austin Steven's Adventures | Curious?: Natural World</t>
+          <t>Pythons 101 | National Geographic</t>
         </is>
       </c>
     </row>
@@ -1017,7 +929,7 @@
     <row r="3">
       <c r="A3" s="18" t="inlineStr">
         <is>
-          <t>2022-06-16</t>
+          <t>2023-09-27</t>
         </is>
       </c>
       <c r="B3" s="20" t="inlineStr">
@@ -1030,113 +942,12 @@
       </c>
       <c r="D3" s="18" t="inlineStr">
         <is>
-          <t>@CuriousNaturalWorld</t>
+          <t>@alexcrowder1673</t>
         </is>
       </c>
       <c r="E3" s="19" t="inlineStr">
         <is>
-          <t>Do you know what Austin's BIGGEST fear is?! Watch as he faces his fears here... 😰 https://youtu.be/TmTx9BmzixQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="18" t="inlineStr">
-        <is>
-          <t>2022-11-06</t>
-        </is>
-      </c>
-      <c r="B4" s="20" t="inlineStr">
-        <is>
-          <t>Negative</t>
-        </is>
-      </c>
-      <c r="C4" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="18" t="inlineStr">
-        <is>
-          <t>@cds3703</t>
-        </is>
-      </c>
-      <c r="E4" s="19" t="inlineStr">
-        <is>
-          <t>dude is scared of spiders but held a fucking king cobra in another episode</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="18" t="inlineStr">
-        <is>
-          <t>2022-08-28</t>
-        </is>
-      </c>
-      <c r="B5" s="20" t="inlineStr">
-        <is>
-          <t>Negative</t>
-        </is>
-      </c>
-      <c r="C5" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="18" t="inlineStr">
-        <is>
-          <t>@mrkipling2201</t>
-        </is>
-      </c>
-      <c r="E5" s="19" t="inlineStr">
-        <is>
-          <t>Red on yellow, kills a fellow.
-Red on black, you’re ok Jack.</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="18" t="inlineStr">
-        <is>
-          <t>2022-06-09</t>
-        </is>
-      </c>
-      <c r="B6" s="20" t="inlineStr">
-        <is>
-          <t>Negative</t>
-        </is>
-      </c>
-      <c r="C6" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="18" t="inlineStr">
-        <is>
-          <t>@rljpdx</t>
-        </is>
-      </c>
-      <c r="E6" s="19" t="inlineStr">
-        <is>
-          <t>that coral snake almost bit as his ass. he decided it was best not to mess with it anymore lol.</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="18" t="inlineStr">
-        <is>
-          <t>2022-06-09</t>
-        </is>
-      </c>
-      <c r="B7" s="20" t="inlineStr">
-        <is>
-          <t>Negative</t>
-        </is>
-      </c>
-      <c r="C7" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" s="18" t="inlineStr">
-        <is>
-          <t>@octavionoelwilliams7450</t>
-        </is>
-      </c>
-      <c r="E7" s="19" t="inlineStr">
-        <is>
-          <t>I remember his show where he was bitten by like 3 of the 7 most deadliest snakes....!!!</t>
+          <t>You guys should honestly hire someone to proof check your videos. National geographic is developing a reputation for being innaccurate.</t>
         </is>
       </c>
     </row>

</xml_diff>